<commit_message>
Actualice el documento comandos HTML
</commit_message>
<xml_diff>
--- a/Cosas Utiles/Comandos git.xlsx
+++ b/Cosas Utiles/Comandos git.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/santosbogo/Documents/Diseño Web/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/santosbogo/Documents/Curso Python Fullstack/Tecnosolidaria/Cosas Utiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19781FA-069B-704F-B96C-40B025E77EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B64A90F3-6F9F-D448-8A03-F5AF58FD02CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="-1880" windowWidth="38400" windowHeight="21600" xr2:uid="{7DACB778-21D6-FC43-B013-925D286B508E}"/>
+    <workbookView xWindow="25600" yWindow="-1380" windowWidth="38400" windowHeight="21100" xr2:uid="{7DACB778-21D6-FC43-B013-925D286B508E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
   <si>
     <t>Comando</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>git checkout &lt;nombre de la rama&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git push </t>
   </si>
 </sst>
 </file>
@@ -553,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C96DEDAA-5E9C-8E46-A779-04A1162BF689}">
-  <dimension ref="B3:E23"/>
+  <dimension ref="B3:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="211" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -744,21 +747,29 @@
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" t="s">
-        <v>30</v>
+      <c r="B22" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="D22" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B23" s="3" t="s">
+      <c r="B23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B24" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D24" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Comence a plasmar en la pagina lo que diseno juli en Excel. Agregue los archivos de imagen de la mano, el logo y la de instagram. Cree un hipervinculo a la pagina de instagram.
</commit_message>
<xml_diff>
--- a/Cosas Utiles/Comandos git.xlsx
+++ b/Cosas Utiles/Comandos git.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/santosbogo/Documents/Curso Python Fullstack/Tecnosolidaria/Cosas Utiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B64A90F3-6F9F-D448-8A03-F5AF58FD02CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8279196-9B79-0541-AA53-63CEE522F983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="-1380" windowWidth="38400" windowHeight="21100" xr2:uid="{7DACB778-21D6-FC43-B013-925D286B508E}"/>
   </bookViews>
@@ -237,11 +237,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -559,7 +560,7 @@
   <dimension ref="B3:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="211" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -642,7 +643,7 @@
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
+      <c r="B10" s="4" t="s">
         <v>34</v>
       </c>
       <c r="D10" t="s">

</xml_diff>